<commit_message>
migration to typescrypte, webpack, yarn, react, etc.
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2235E18-BF70-44C0-B229-8DAE2C97440F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23288707-9960-4981-BFD0-2293171F234A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2490" yWindow="3645" windowWidth="18900" windowHeight="13500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1635" yWindow="4695" windowWidth="18900" windowHeight="13500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="18">
   <si>
     <t>FI0001</t>
   </si>
@@ -74,9 +74,6 @@
   </si>
   <si>
     <t>G06</t>
-  </si>
-  <si>
-    <t>G07</t>
   </si>
 </sst>
 </file>
@@ -394,100 +391,204 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D7:I14"/>
+  <dimension ref="B2:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="7" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
       <c r="E7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>7</v>
       </c>
-      <c r="F7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H7" t="s">
-        <v>10</v>
-      </c>
-      <c r="I7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="C15" t="s">
         <v>12</v>
       </c>
-      <c r="G8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" t="s">
+      <c r="D15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D9" t="s">
+      <c r="G15" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" t="s">
         <v>1</v>
       </c>
-      <c r="E9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D10" t="s">
+      <c r="E17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" t="s">
         <v>2</v>
       </c>
-      <c r="E10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="G18" t="s">
+        <v>5</v>
+      </c>
+      <c r="H18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D12" t="s">
-        <v>4</v>
-      </c>
-      <c r="E12" t="s">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D13" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" t="s">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>